<commit_message>
Corrected PCB rev callout (0.2c)
</commit_message>
<xml_diff>
--- a/PCB/v0.2c/TeensyROM v0.2c BOM.xlsx
+++ b/PCB/v0.2c/TeensyROM v0.2c BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyData\Geek Stuff\Projects\Commodore 64\Hardware\Expansion Port\TeensyROM\TeensyROM\PCB\v0.2c\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA9D520-C959-4D35-91E3-CED8BAE4F785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D14D3C9-0229-4ADD-A97C-B2F7C143242D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{5596D14A-B5AE-4503-9066-038068479CCD}"/>
+    <workbookView xWindow="1584" yWindow="648" windowWidth="21456" windowHeight="12312" xr2:uid="{5596D14A-B5AE-4503-9066-038068479CCD}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="2" r:id="rId1"/>
@@ -602,9 +602,6 @@
     <t>Locations/RefDes</t>
   </si>
   <si>
-    <t>TeensyROM v0.2b</t>
-  </si>
-  <si>
     <t>SN74LVC07ADR
 MC74LCX07</t>
   </si>
@@ -710,6 +707,9 @@
   </si>
   <si>
     <t>1 hour labor</t>
+  </si>
+  <si>
+    <t>TeensyROM v0.2c</t>
   </si>
 </sst>
 </file>
@@ -959,7 +959,6 @@
     <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -998,6 +997,9 @@
     </xf>
     <xf numFmtId="44" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1318,8 +1320,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1"/>
@@ -1383,10 +1385,10 @@
         <v>105</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="F2" s="34" t="s">
-        <v>175</v>
+        <v>178</v>
+      </c>
+      <c r="F2" s="47" t="s">
+        <v>204</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>135</v>
@@ -1400,7 +1402,7 @@
         <v>10.799999999999999</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1411,7 +1413,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>137</v>
@@ -1442,7 +1444,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>171</v>
@@ -1473,7 +1475,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>136</v>
@@ -1543,13 +1545,13 @@
         <v>139</v>
       </c>
       <c r="E7" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>175</v>
+      </c>
+      <c r="G7" s="13" t="s">
         <v>177</v>
-      </c>
-      <c r="F7" s="27" t="s">
-        <v>176</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>178</v>
       </c>
       <c r="H7" s="20">
         <v>0.5</v>
@@ -1559,7 +1561,7 @@
         <v>0.5</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="43.2">
@@ -1592,7 +1594,7 @@
         <v>33.08</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="28.8">
@@ -1658,7 +1660,7 @@
         <v>0.26</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="28.8">
@@ -1691,7 +1693,7 @@
         <v>0.19</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1755,7 +1757,7 @@
         <v>0.43</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="28.8">
@@ -1769,7 +1771,7 @@
         <v>20</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>147</v>
@@ -1868,16 +1870,16 @@
         <v>128</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E17" s="16" t="s">
         <v>170</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H17" s="20">
         <v>0.74</v>
@@ -1892,25 +1894,25 @@
     </row>
     <row r="18" spans="1:10" ht="28.8">
       <c r="A18" s="15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B18" s="5">
         <v>1</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>193</v>
       </c>
       <c r="E18" s="16" t="s">
         <v>170</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H18" s="20">
         <v>0.2</v>
@@ -1922,176 +1924,176 @@
       <c r="J18" s="6"/>
     </row>
     <row r="19" spans="1:10" hidden="1" outlineLevel="1">
-      <c r="A19" s="44">
+      <c r="A19" s="43">
         <v>17</v>
       </c>
-      <c r="B19" s="35">
+      <c r="B19" s="34">
         <v>2</v>
       </c>
-      <c r="C19" s="35" t="s">
+      <c r="C19" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="D19" s="36" t="s">
+      <c r="D19" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="35" t="s">
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="34" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" hidden="1" outlineLevel="1">
+      <c r="A20" s="43">
+        <v>18</v>
+      </c>
+      <c r="B20" s="34">
+        <v>1</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>119</v>
+      </c>
+      <c r="D20" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="34" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="20" spans="1:10" hidden="1" outlineLevel="1">
-      <c r="A20" s="44">
-        <v>18</v>
-      </c>
-      <c r="B20" s="35">
-        <v>1</v>
-      </c>
-      <c r="C20" s="35" t="s">
-        <v>119</v>
-      </c>
-      <c r="D20" s="36" t="s">
-        <v>117</v>
-      </c>
-      <c r="E20" s="35"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="37"/>
-      <c r="J20" s="35" t="s">
+    <row r="21" spans="1:10" hidden="1" outlineLevel="1">
+      <c r="A21" s="43">
+        <v>19</v>
+      </c>
+      <c r="B21" s="34">
+        <v>1</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="E21" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="F21" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="G21" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="H21" s="36"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="34" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="21" spans="1:10" hidden="1" outlineLevel="1">
-      <c r="A21" s="44">
-        <v>19</v>
-      </c>
-      <c r="B21" s="35">
-        <v>1</v>
-      </c>
-      <c r="C21" s="35" t="s">
-        <v>120</v>
-      </c>
-      <c r="D21" s="35" t="s">
-        <v>109</v>
-      </c>
-      <c r="E21" s="35" t="s">
-        <v>110</v>
-      </c>
-      <c r="F21" s="35" t="s">
-        <v>111</v>
-      </c>
-      <c r="G21" s="35" t="s">
-        <v>112</v>
-      </c>
-      <c r="H21" s="37"/>
-      <c r="I21" s="37"/>
-      <c r="J21" s="35" t="s">
+    <row r="22" spans="1:10" hidden="1" outlineLevel="1">
+      <c r="A22" s="43">
+        <v>20</v>
+      </c>
+      <c r="B22" s="34">
+        <v>1</v>
+      </c>
+      <c r="C22" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="D22" s="34" t="s">
+        <v>186</v>
+      </c>
+      <c r="E22" s="37" t="s">
+        <v>148</v>
+      </c>
+      <c r="F22" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="G22" s="34"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="34" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="22" spans="1:10" hidden="1" outlineLevel="1">
-      <c r="A22" s="44">
-        <v>20</v>
-      </c>
-      <c r="B22" s="35">
-        <v>1</v>
-      </c>
-      <c r="C22" s="35" t="s">
-        <v>125</v>
-      </c>
-      <c r="D22" s="35" t="s">
-        <v>187</v>
-      </c>
-      <c r="E22" s="38" t="s">
+    <row r="23" spans="1:10" hidden="1" outlineLevel="1">
+      <c r="A23" s="43">
+        <v>21</v>
+      </c>
+      <c r="B23" s="34">
+        <v>1</v>
+      </c>
+      <c r="C23" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="D23" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="E23" s="37" t="s">
         <v>148</v>
       </c>
-      <c r="F22" s="35" t="s">
-        <v>124</v>
-      </c>
-      <c r="G22" s="35"/>
-      <c r="H22" s="37"/>
-      <c r="I22" s="37"/>
-      <c r="J22" s="35" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" hidden="1" outlineLevel="1">
-      <c r="A23" s="44">
-        <v>21</v>
-      </c>
-      <c r="B23" s="35">
-        <v>1</v>
-      </c>
-      <c r="C23" s="35" t="s">
-        <v>126</v>
-      </c>
-      <c r="D23" s="35" t="s">
-        <v>122</v>
-      </c>
-      <c r="E23" s="38" t="s">
-        <v>148</v>
-      </c>
-      <c r="F23" s="35" t="s">
+      <c r="F23" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="G23" s="35"/>
-      <c r="H23" s="37"/>
-      <c r="I23" s="37"/>
-      <c r="J23" s="35" t="s">
-        <v>186</v>
+      <c r="G23" s="34"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="36"/>
+      <c r="J23" s="34" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="24" spans="1:10" hidden="1" outlineLevel="1">
-      <c r="A24" s="43">
+      <c r="A24" s="42">
         <v>23</v>
       </c>
-      <c r="B24" s="39">
-        <v>1</v>
-      </c>
-      <c r="C24" s="40" t="s">
+      <c r="B24" s="38">
+        <v>1</v>
+      </c>
+      <c r="C24" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="D24" s="42" t="s">
-        <v>203</v>
-      </c>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="41"/>
-      <c r="I24" s="41"/>
-      <c r="J24" s="40" t="s">
+      <c r="D24" s="41" t="s">
+        <v>202</v>
+      </c>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="39" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:10" hidden="1" outlineLevel="1">
-      <c r="A25" s="43">
+      <c r="A25" s="42">
         <v>24</v>
       </c>
-      <c r="B25" s="39">
-        <v>1</v>
-      </c>
-      <c r="C25" s="40" t="s">
+      <c r="B25" s="38">
+        <v>1</v>
+      </c>
+      <c r="C25" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="D25" s="40" t="s">
+      <c r="D25" s="39" t="s">
         <v>141</v>
       </c>
-      <c r="E25" s="40"/>
-      <c r="F25" s="40"/>
-      <c r="G25" s="40"/>
-      <c r="H25" s="41"/>
-      <c r="I25" s="41"/>
-      <c r="J25" s="40" t="s">
+      <c r="E25" s="39"/>
+      <c r="F25" s="39"/>
+      <c r="G25" s="39"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="39" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:10" s="30" customFormat="1" ht="13.8" customHeight="1" collapsed="1">
-      <c r="A26" s="45"/>
-      <c r="B26" s="46"/>
+      <c r="A26" s="44"/>
+      <c r="B26" s="45"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
@@ -2136,14 +2138,14 @@
         <v>15</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="31" spans="1:10">
-      <c r="G31" s="47" t="s">
+      <c r="G31" s="46" t="s">
         <v>164</v>
       </c>
-      <c r="H31" s="47"/>
+      <c r="H31" s="46"/>
       <c r="I31" s="23">
         <f>I30+I29</f>
         <v>79.305999999999997</v>

</xml_diff>

<commit_message>
Corrected schematic value of 74LVC245, was listed as 74LCV245
</commit_message>
<xml_diff>
--- a/PCB/v0.2c/TeensyROM v0.2c BOM.xlsx
+++ b/PCB/v0.2c/TeensyROM v0.2c BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyData\Geek Stuff\Projects\Commodore 64\Hardware\Expansion Port\TeensyROM\TeensyROM\PCB\v0.2c\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D14D3C9-0229-4ADD-A97C-B2F7C143242D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC11906E-2217-4945-AF66-3333A4E64400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1584" yWindow="648" windowWidth="21456" windowHeight="12312" xr2:uid="{5596D14A-B5AE-4503-9066-038068479CCD}"/>
+    <workbookView xWindow="4230" yWindow="-13650" windowWidth="21480" windowHeight="12330" xr2:uid="{5596D14A-B5AE-4503-9066-038068479CCD}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="2" r:id="rId1"/>
@@ -463,9 +463,6 @@
     <t>RES 0805 1K</t>
   </si>
   <si>
-    <t>74LCV245, SO20W/N</t>
-  </si>
-  <si>
     <t>74LVC07, SO14</t>
   </si>
   <si>
@@ -710,6 +707,9 @@
   </si>
   <si>
     <t>TeensyROM v0.2c</t>
+  </si>
+  <si>
+    <t>74LVC245, SO20W/N</t>
   </si>
 </sst>
 </file>
@@ -995,11 +995,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="44" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1321,7 +1321,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1"/>
@@ -1347,7 +1347,7 @@
         <v>18</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>0</v>
@@ -1356,13 +1356,13 @@
         <v>29</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I1" s="17" t="s">
         <v>130</v>
@@ -1385,10 +1385,10 @@
         <v>105</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="F2" s="47" t="s">
-        <v>204</v>
+        <v>177</v>
+      </c>
+      <c r="F2" s="46" t="s">
+        <v>203</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>135</v>
@@ -1402,7 +1402,7 @@
         <v>10.799999999999999</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1413,7 +1413,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>137</v>
@@ -1444,19 +1444,19 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>133</v>
       </c>
       <c r="F4" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="G4" s="13" t="s">
         <v>172</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>173</v>
       </c>
       <c r="H4" s="20">
         <v>0.1</v>
@@ -1475,19 +1475,19 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>136</v>
       </c>
       <c r="E5" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="G5" s="24" t="s">
         <v>143</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="G5" s="24" t="s">
-        <v>144</v>
       </c>
       <c r="H5" s="21">
         <v>0.1</v>
@@ -1509,7 +1509,7 @@
         <v>23</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>138</v>
+        <v>204</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>106</v>
@@ -1528,7 +1528,7 @@
         <v>2.72</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="28.8">
@@ -1542,16 +1542,16 @@
         <v>17</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E7" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="G7" s="13" t="s">
         <v>176</v>
-      </c>
-      <c r="F7" s="27" t="s">
-        <v>175</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>177</v>
       </c>
       <c r="H7" s="20">
         <v>0.5</v>
@@ -1561,7 +1561,7 @@
         <v>0.5</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="43.2">
@@ -1578,7 +1578,7 @@
         <v>121</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F8" s="26" t="s">
         <v>13</v>
@@ -1594,7 +1594,7 @@
         <v>33.08</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="28.8">
@@ -1608,16 +1608,16 @@
         <v>103</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E9" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="F9" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="F9" s="8" t="s">
-        <v>154</v>
-      </c>
       <c r="G9" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H9" s="20">
         <v>1.31</v>
@@ -1641,16 +1641,16 @@
         <v>102</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F10" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="G10" s="13" t="s">
         <v>158</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>159</v>
       </c>
       <c r="H10" s="20">
         <v>0.26</v>
@@ -1660,7 +1660,7 @@
         <v>0.26</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="28.8">
@@ -1674,13 +1674,13 @@
         <v>104</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>110</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G11" s="13" t="s">
         <v>38</v>
@@ -1693,7 +1693,7 @@
         <v>0.19</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1707,7 +1707,7 @@
         <v>42</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>31</v>
@@ -1757,7 +1757,7 @@
         <v>0.43</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="28.8">
@@ -1771,16 +1771,16 @@
         <v>20</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H14" s="20">
         <v>0.22</v>
@@ -1790,7 +1790,7 @@
         <v>0.44</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1870,16 +1870,16 @@
         <v>128</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H17" s="20">
         <v>0.74</v>
@@ -1894,25 +1894,25 @@
     </row>
     <row r="18" spans="1:10" ht="28.8">
       <c r="A18" s="15" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B18" s="5">
         <v>1</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="F18" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="E18" s="16" t="s">
-        <v>170</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>193</v>
-      </c>
       <c r="G18" s="13" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H18" s="20">
         <v>0.2</v>
@@ -1942,7 +1942,7 @@
       <c r="H19" s="36"/>
       <c r="I19" s="36"/>
       <c r="J19" s="34" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="20" spans="1:10" hidden="1" outlineLevel="1">
@@ -1964,7 +1964,7 @@
       <c r="H20" s="36"/>
       <c r="I20" s="36"/>
       <c r="J20" s="34" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="21" spans="1:10" hidden="1" outlineLevel="1">
@@ -1992,7 +1992,7 @@
       <c r="H21" s="36"/>
       <c r="I21" s="36"/>
       <c r="J21" s="34" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="22" spans="1:10" hidden="1" outlineLevel="1">
@@ -2006,10 +2006,10 @@
         <v>125</v>
       </c>
       <c r="D22" s="34" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E22" s="37" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F22" s="34" t="s">
         <v>124</v>
@@ -2018,7 +2018,7 @@
       <c r="H22" s="36"/>
       <c r="I22" s="36"/>
       <c r="J22" s="34" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="23" spans="1:10" hidden="1" outlineLevel="1">
@@ -2035,7 +2035,7 @@
         <v>122</v>
       </c>
       <c r="E23" s="37" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F23" s="34" t="s">
         <v>123</v>
@@ -2044,7 +2044,7 @@
       <c r="H23" s="36"/>
       <c r="I23" s="36"/>
       <c r="J23" s="34" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="24" spans="1:10" hidden="1" outlineLevel="1">
@@ -2058,7 +2058,7 @@
         <v>83</v>
       </c>
       <c r="D24" s="41" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E24" s="39"/>
       <c r="F24" s="39"/>
@@ -2080,7 +2080,7 @@
         <v>54</v>
       </c>
       <c r="D25" s="39" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E25" s="39"/>
       <c r="F25" s="39"/>
@@ -2105,7 +2105,7 @@
     </row>
     <row r="27" spans="1:10">
       <c r="H27" s="19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I27" s="28">
         <f>SUM(I2:I25)</f>
@@ -2114,7 +2114,7 @@
     </row>
     <row r="28" spans="1:10">
       <c r="H28" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I28" s="18">
         <f>I27*10%</f>
@@ -2123,7 +2123,7 @@
     </row>
     <row r="29" spans="1:10">
       <c r="H29" s="22" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I29" s="23">
         <f>I28+I27</f>
@@ -2132,20 +2132,20 @@
     </row>
     <row r="30" spans="1:10">
       <c r="H30" s="32" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I30" s="18">
         <v>15</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="31" spans="1:10">
-      <c r="G31" s="46" t="s">
-        <v>164</v>
-      </c>
-      <c r="H31" s="46"/>
+      <c r="G31" s="47" t="s">
+        <v>163</v>
+      </c>
+      <c r="H31" s="47"/>
       <c r="I31" s="23">
         <f>I30+I29</f>
         <v>79.305999999999997</v>
@@ -2154,10 +2154,10 @@
     <row r="32" spans="1:10">
       <c r="G32" s="29"/>
       <c r="H32" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="I32" s="22" t="s">
         <v>165</v>
-      </c>
-      <c r="I32" s="22" t="s">
-        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Heatsink info updated in BOM
</commit_message>
<xml_diff>
--- a/PCB/v0.2c/TeensyROM v0.2c BOM.xlsx
+++ b/PCB/v0.2c/TeensyROM v0.2c BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyData\Geek Stuff\Projects\Commodore 64\Hardware\Expansion Port\TeensyROM\TeensyROM\PCB\v0.2c\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC11906E-2217-4945-AF66-3333A4E64400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A775DD3-119E-4535-8DA2-BCEBF619239F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4230" yWindow="-13650" windowWidth="21480" windowHeight="12330" xr2:uid="{5596D14A-B5AE-4503-9066-038068479CCD}"/>
+    <workbookView xWindow="-30" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{5596D14A-B5AE-4503-9066-038068479CCD}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="207">
   <si>
     <t>Value</t>
   </si>
@@ -434,9 +434,6 @@
   </si>
   <si>
     <t>U1 Heatsink</t>
-  </si>
-  <si>
-    <t>Optional, but recommended</t>
   </si>
   <si>
     <t>Extended Cost (USD)</t>
@@ -648,9 +645,6 @@
 Recommend ENIG finish, 30° chamfered gold fingers, Purple solder mask</t>
   </si>
   <si>
-    <t>AE11386-ND</t>
-  </si>
-  <si>
     <t>U1 Therm Pad</t>
   </si>
   <si>
@@ -661,16 +655,10 @@
 TG-T1000-11-11-0.25-5PT</t>
   </si>
   <si>
-    <t>Assmann V2019B</t>
-  </si>
-  <si>
     <t>1168-TG-T1000-11-11-0.25-5PT-ND</t>
   </si>
   <si>
     <t>16a</t>
-  </si>
-  <si>
-    <t>12x12mm Aluminum heatsink</t>
   </si>
   <si>
     <t>22uF, 16-25v CPOL-US E2.5-6
@@ -710,6 +698,28 @@
   </si>
   <si>
     <t>74LVC245, SO20W/N</t>
+  </si>
+  <si>
+    <t>B0B7K2TWZM</t>
+  </si>
+  <si>
+    <t>If needed (recommended heatsink has thermal pad included)</t>
+  </si>
+  <si>
+    <t>Jeteokar</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B0B7K2TWZM   or 
+https://www.ebay.com/itm/115401351474</t>
+  </si>
+  <si>
+    <t>12x12mm Aluminum heatsink
+w/ thermal tape attached
+Max height to fit in case: ~15mm</t>
+  </si>
+  <si>
+    <t>Optional, but recommended
+Can sub other 12x12mm heatsinks/pads</t>
   </si>
 </sst>
 </file>
@@ -862,7 +872,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -998,8 +1008,14 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="44" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1321,7 +1337,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1"/>
@@ -1347,7 +1363,7 @@
         <v>18</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>0</v>
@@ -1356,16 +1372,16 @@
         <v>29</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I1" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J1" s="10" t="s">
         <v>25</v>
@@ -1385,13 +1401,13 @@
         <v>105</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F2" s="46" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H2" s="20">
         <f>32.4/3</f>
@@ -1402,7 +1418,7 @@
         <v>10.799999999999999</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1413,19 +1429,19 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E3" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="G3" s="13" t="s">
         <v>133</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>134</v>
       </c>
       <c r="H3" s="20">
         <v>0.1</v>
@@ -1444,19 +1460,19 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="F4" s="6" t="s">
+      <c r="G4" s="13" t="s">
         <v>171</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>172</v>
       </c>
       <c r="H4" s="20">
         <v>0.1</v>
@@ -1475,19 +1491,19 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E5" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="G5" s="24" t="s">
         <v>142</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="G5" s="24" t="s">
-        <v>143</v>
       </c>
       <c r="H5" s="21">
         <v>0.1</v>
@@ -1509,7 +1525,7 @@
         <v>23</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>106</v>
@@ -1528,7 +1544,7 @@
         <v>2.72</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="28.8">
@@ -1542,16 +1558,16 @@
         <v>17</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E7" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="G7" s="13" t="s">
         <v>175</v>
-      </c>
-      <c r="F7" s="27" t="s">
-        <v>174</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>176</v>
       </c>
       <c r="H7" s="20">
         <v>0.5</v>
@@ -1561,7 +1577,7 @@
         <v>0.5</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="43.2">
@@ -1578,13 +1594,13 @@
         <v>121</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F8" s="26" t="s">
         <v>13</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H8" s="20">
         <v>33.08</v>
@@ -1594,7 +1610,7 @@
         <v>33.08</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="28.8">
@@ -1608,16 +1624,16 @@
         <v>103</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E9" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="F9" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="F9" s="8" t="s">
-        <v>153</v>
-      </c>
       <c r="G9" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H9" s="20">
         <v>1.31</v>
@@ -1641,16 +1657,16 @@
         <v>102</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F10" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="G10" s="13" t="s">
         <v>157</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>158</v>
       </c>
       <c r="H10" s="20">
         <v>0.26</v>
@@ -1660,7 +1676,7 @@
         <v>0.26</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="28.8">
@@ -1674,13 +1690,13 @@
         <v>104</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>110</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G11" s="13" t="s">
         <v>38</v>
@@ -1693,7 +1709,7 @@
         <v>0.19</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1707,7 +1723,7 @@
         <v>42</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>31</v>
@@ -1757,7 +1773,7 @@
         <v>0.43</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="28.8">
@@ -1771,16 +1787,16 @@
         <v>20</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H14" s="20">
         <v>0.22</v>
@@ -1790,7 +1806,7 @@
         <v>0.44</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1859,7 +1875,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="28.8">
+    <row r="17" spans="1:10" ht="57.6">
       <c r="A17" s="15">
         <v>16</v>
       </c>
@@ -1870,49 +1886,50 @@
         <v>128</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>169</v>
+        <v>205</v>
+      </c>
+      <c r="E17" s="47" t="s">
+        <v>203</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="G17" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="G17" s="49" t="s">
+        <v>204</v>
+      </c>
+      <c r="H17" s="20">
+        <f>9.98/20</f>
+        <v>0.499</v>
+      </c>
+      <c r="I17" s="20">
+        <f t="shared" si="2"/>
+        <v>0.499</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="28.8" hidden="1">
+      <c r="A18" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="B18" s="5">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="H17" s="20">
-        <v>0.74</v>
-      </c>
-      <c r="I17" s="20">
-        <f>H17*B17</f>
-        <v>0.74</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="28.8">
-      <c r="A18" s="15" t="s">
-        <v>195</v>
-      </c>
-      <c r="B18" s="5">
-        <v>1</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="E18" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="F18" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="G18" s="13" t="s">
         <v>191</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>169</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>194</v>
       </c>
       <c r="H18" s="20">
         <v>0.2</v>
@@ -1921,7 +1938,9 @@
         <f t="shared" si="2"/>
         <v>0.2</v>
       </c>
-      <c r="J18" s="6"/>
+      <c r="J18" s="6" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="19" spans="1:10" hidden="1" outlineLevel="1">
       <c r="A19" s="43">
@@ -1942,7 +1961,7 @@
       <c r="H19" s="36"/>
       <c r="I19" s="36"/>
       <c r="J19" s="34" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="20" spans="1:10" hidden="1" outlineLevel="1">
@@ -1964,7 +1983,7 @@
       <c r="H20" s="36"/>
       <c r="I20" s="36"/>
       <c r="J20" s="34" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="21" spans="1:10" hidden="1" outlineLevel="1">
@@ -1992,7 +2011,7 @@
       <c r="H21" s="36"/>
       <c r="I21" s="36"/>
       <c r="J21" s="34" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="22" spans="1:10" hidden="1" outlineLevel="1">
@@ -2006,10 +2025,10 @@
         <v>125</v>
       </c>
       <c r="D22" s="34" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E22" s="37" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F22" s="34" t="s">
         <v>124</v>
@@ -2018,7 +2037,7 @@
       <c r="H22" s="36"/>
       <c r="I22" s="36"/>
       <c r="J22" s="34" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="23" spans="1:10" hidden="1" outlineLevel="1">
@@ -2035,7 +2054,7 @@
         <v>122</v>
       </c>
       <c r="E23" s="37" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F23" s="34" t="s">
         <v>123</v>
@@ -2044,7 +2063,7 @@
       <c r="H23" s="36"/>
       <c r="I23" s="36"/>
       <c r="J23" s="34" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="24" spans="1:10" hidden="1" outlineLevel="1">
@@ -2058,7 +2077,7 @@
         <v>83</v>
       </c>
       <c r="D24" s="41" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E24" s="39"/>
       <c r="F24" s="39"/>
@@ -2080,7 +2099,7 @@
         <v>54</v>
       </c>
       <c r="D25" s="39" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E25" s="39"/>
       <c r="F25" s="39"/>
@@ -2105,59 +2124,59 @@
     </row>
     <row r="27" spans="1:10">
       <c r="H27" s="19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I27" s="28">
         <f>SUM(I2:I25)</f>
-        <v>58.459999999999994</v>
+        <v>58.218999999999994</v>
       </c>
     </row>
     <row r="28" spans="1:10">
       <c r="H28" s="32" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I28" s="18">
         <f>I27*10%</f>
-        <v>5.8460000000000001</v>
+        <v>5.8218999999999994</v>
       </c>
     </row>
     <row r="29" spans="1:10">
       <c r="H29" s="22" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I29" s="23">
         <f>I28+I27</f>
-        <v>64.305999999999997</v>
+        <v>64.040899999999993</v>
       </c>
     </row>
     <row r="30" spans="1:10">
       <c r="H30" s="32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I30" s="18">
         <v>15</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="31" spans="1:10">
-      <c r="G31" s="47" t="s">
-        <v>163</v>
-      </c>
-      <c r="H31" s="47"/>
+      <c r="G31" s="48" t="s">
+        <v>162</v>
+      </c>
+      <c r="H31" s="48"/>
       <c r="I31" s="23">
         <f>I30+I29</f>
-        <v>79.305999999999997</v>
+        <v>79.040899999999993</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="G32" s="29"/>
       <c r="H32" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="I32" s="22" t="s">
         <v>164</v>
-      </c>
-      <c r="I32" s="22" t="s">
-        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -2167,30 +2186,28 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E8" r:id="rId1" display="https://www.pjrc.com/store" xr:uid="{134792E2-B64E-4FBB-BFC7-EC447106886D}"/>
-    <hyperlink ref="E17" r:id="rId2" xr:uid="{5FD644F6-19A2-4D0C-BDC2-C003DADB325A}"/>
-    <hyperlink ref="G6" r:id="rId3" display="https://www.digikey.com/en/products/detail/nexperia-usa-inc/74LVC245AD-118/946690" xr:uid="{58DCABB5-EDC7-4E2D-A244-D34D14A1826B}"/>
-    <hyperlink ref="F8" r:id="rId4" xr:uid="{8F740FC1-EDF0-4C9E-9823-C987C0E04A4F}"/>
-    <hyperlink ref="G8" r:id="rId5" xr:uid="{0DE6FCC4-E35A-47FB-9DC7-F030B4E296C0}"/>
-    <hyperlink ref="G7" r:id="rId6" display="296-8441-1-ND" xr:uid="{E5BB0DA3-B914-4FF4-B66E-5980E82AA257}"/>
-    <hyperlink ref="G3" r:id="rId7" xr:uid="{D713217F-486F-4E73-A804-2166CA542C2D}"/>
-    <hyperlink ref="G5" r:id="rId8" xr:uid="{00640734-08BA-4F39-8C8E-D0CF6E96C735}"/>
-    <hyperlink ref="G12" r:id="rId9" xr:uid="{6F229ED7-CAEA-4D67-BFF0-0E0AA066F8B2}"/>
-    <hyperlink ref="G13" r:id="rId10" xr:uid="{FE4A259F-8D56-43F3-928F-E2509BF332B9}"/>
-    <hyperlink ref="G14" r:id="rId11" xr:uid="{5AA0053B-4694-45A0-990D-299A2E63F143}"/>
-    <hyperlink ref="G15" r:id="rId12" xr:uid="{B7489C6B-4B67-493F-A4BC-72AA11902DA0}"/>
-    <hyperlink ref="G16" r:id="rId13" xr:uid="{0F65CBF2-C3AE-4742-BDAA-ADF047E394C6}"/>
-    <hyperlink ref="G11" r:id="rId14" xr:uid="{4E963CB5-4BC8-4A66-A683-2D131B96C08C}"/>
-    <hyperlink ref="G9" r:id="rId15" xr:uid="{890A73F3-E6DD-4DD6-A06E-81924A5413A3}"/>
-    <hyperlink ref="G10" r:id="rId16" xr:uid="{DF130F23-5B34-41D1-86C6-D27E2C2FCFE8}"/>
-    <hyperlink ref="G17" r:id="rId17" xr:uid="{E52F636D-3699-4616-A972-2410D7682974}"/>
-    <hyperlink ref="G4" r:id="rId18" xr:uid="{BFF33686-00DA-47D6-B57E-31FEFD3C8B56}"/>
-    <hyperlink ref="E22" r:id="rId19" display="https://www.pjrc.com/store" xr:uid="{4CF63453-125C-408F-8E09-8A412D6E1A65}"/>
-    <hyperlink ref="E23" r:id="rId20" display="https://www.pjrc.com/store" xr:uid="{AFCDA104-AF2B-4C61-8019-A6A0C8B60F5C}"/>
-    <hyperlink ref="E18" r:id="rId21" xr:uid="{90126B75-8BEB-424E-8FE0-DEBACDA6E296}"/>
-    <hyperlink ref="G18" r:id="rId22" display="https://www.digikey.com/en/products/detail/t-global-technology/TG-T1000-11-11-0-25-5PT/13919490" xr:uid="{2859B1F5-9DA9-47E4-8E21-91710442DAD7}"/>
+    <hyperlink ref="G6" r:id="rId2" display="https://www.digikey.com/en/products/detail/nexperia-usa-inc/74LVC245AD-118/946690" xr:uid="{58DCABB5-EDC7-4E2D-A244-D34D14A1826B}"/>
+    <hyperlink ref="F8" r:id="rId3" xr:uid="{8F740FC1-EDF0-4C9E-9823-C987C0E04A4F}"/>
+    <hyperlink ref="G8" r:id="rId4" xr:uid="{0DE6FCC4-E35A-47FB-9DC7-F030B4E296C0}"/>
+    <hyperlink ref="G7" r:id="rId5" display="296-8441-1-ND" xr:uid="{E5BB0DA3-B914-4FF4-B66E-5980E82AA257}"/>
+    <hyperlink ref="G3" r:id="rId6" xr:uid="{D713217F-486F-4E73-A804-2166CA542C2D}"/>
+    <hyperlink ref="G5" r:id="rId7" xr:uid="{00640734-08BA-4F39-8C8E-D0CF6E96C735}"/>
+    <hyperlink ref="G12" r:id="rId8" xr:uid="{6F229ED7-CAEA-4D67-BFF0-0E0AA066F8B2}"/>
+    <hyperlink ref="G13" r:id="rId9" xr:uid="{FE4A259F-8D56-43F3-928F-E2509BF332B9}"/>
+    <hyperlink ref="G14" r:id="rId10" xr:uid="{5AA0053B-4694-45A0-990D-299A2E63F143}"/>
+    <hyperlink ref="G15" r:id="rId11" xr:uid="{B7489C6B-4B67-493F-A4BC-72AA11902DA0}"/>
+    <hyperlink ref="G16" r:id="rId12" xr:uid="{0F65CBF2-C3AE-4742-BDAA-ADF047E394C6}"/>
+    <hyperlink ref="G11" r:id="rId13" xr:uid="{4E963CB5-4BC8-4A66-A683-2D131B96C08C}"/>
+    <hyperlink ref="G9" r:id="rId14" xr:uid="{890A73F3-E6DD-4DD6-A06E-81924A5413A3}"/>
+    <hyperlink ref="G10" r:id="rId15" xr:uid="{DF130F23-5B34-41D1-86C6-D27E2C2FCFE8}"/>
+    <hyperlink ref="G4" r:id="rId16" xr:uid="{BFF33686-00DA-47D6-B57E-31FEFD3C8B56}"/>
+    <hyperlink ref="E22" r:id="rId17" display="https://www.pjrc.com/store" xr:uid="{4CF63453-125C-408F-8E09-8A412D6E1A65}"/>
+    <hyperlink ref="E23" r:id="rId18" display="https://www.pjrc.com/store" xr:uid="{AFCDA104-AF2B-4C61-8019-A6A0C8B60F5C}"/>
+    <hyperlink ref="E18" r:id="rId19" xr:uid="{90126B75-8BEB-424E-8FE0-DEBACDA6E296}"/>
+    <hyperlink ref="G18" r:id="rId20" display="https://www.digikey.com/en/products/detail/t-global-technology/TG-T1000-11-11-0-25-5PT/13919490" xr:uid="{2859B1F5-9DA9-47E4-8E21-91710442DAD7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId23"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId21"/>
 </worksheet>
 </file>
 

</xml_diff>